<commit_message>
preenchimento da tabela de dados
</commit_message>
<xml_diff>
--- a/insertData.xlsx
+++ b/insertData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luana.scardua\Downloads\SQLite-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Meu Drive\2021-2_LP2\trabalhoLP2\kPython-SQLite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CC5882-366A-4A8B-B41B-6FAFAA5178A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE6EAFB-C04B-450F-AF07-8A990263E57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6CFF9A66-05E6-4823-8BFA-658619B48BFB}"/>
+    <workbookView xWindow="46170" yWindow="2850" windowWidth="16065" windowHeight="12315" activeTab="3" xr2:uid="{6CFF9A66-05E6-4823-8BFA-658619B48BFB}"/>
   </bookViews>
   <sheets>
     <sheet name="usuario" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>id</t>
   </si>
@@ -89,13 +89,124 @@
   </si>
   <si>
     <t>PROJ</t>
+  </si>
+  <si>
+    <t>Andre Almeida</t>
+  </si>
+  <si>
+    <t>PROF</t>
+  </si>
+  <si>
+    <t>Bruno Bento</t>
+  </si>
+  <si>
+    <t>Carla Caetano</t>
+  </si>
+  <si>
+    <t>Dora Donato</t>
+  </si>
+  <si>
+    <t>Ella Escobar</t>
+  </si>
+  <si>
+    <t>PRV</t>
+  </si>
+  <si>
+    <t>Prova</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>SEM01</t>
+  </si>
+  <si>
+    <t>PROJ2</t>
+  </si>
+  <si>
+    <t>PRV01</t>
+  </si>
+  <si>
+    <t>Prova do 1º bimestre</t>
+  </si>
+  <si>
+    <t>Projeto sobre luz</t>
+  </si>
+  <si>
+    <t>Seminário em grupo</t>
+  </si>
+  <si>
+    <t>PRV02</t>
+  </si>
+  <si>
+    <t>Prova do 2º bimestre</t>
+  </si>
+  <si>
+    <t>PRV1</t>
+  </si>
+  <si>
+    <t>Prova final</t>
+  </si>
+  <si>
+    <t>idUser</t>
+  </si>
+  <si>
+    <t>idAvaliacao</t>
+  </si>
+  <si>
+    <t>dataConclusao</t>
+  </si>
+  <si>
+    <t>notaAtribuida</t>
+  </si>
+  <si>
+    <t>situacao</t>
+  </si>
+  <si>
+    <t>Fernada Ferreira</t>
+  </si>
+  <si>
+    <t>Gisele Gente</t>
+  </si>
+  <si>
+    <t>Heitor Hera</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>aprovado</t>
+  </si>
+  <si>
+    <t>reprovado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -106,6 +217,19 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -130,13 +254,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,18 +579,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F016AF-984E-4592-8A35-D09FFCDCC7C2}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C16" sqref="C16:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -490,7 +618,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -498,6 +626,94 @@
         <v>6</v>
       </c>
       <c r="D3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
         <v>14</v>
       </c>
     </row>
@@ -509,15 +725,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F405A2-8FE6-4448-B6F8-DFECE18E1EBE}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -525,7 +741,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -533,12 +749,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -549,80 +773,426 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E4AC80-24BD-4308-9E1D-510E74F54FEE}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="27.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="E2" s="3">
         <v>44256</v>
       </c>
-      <c r="D2" s="3">
+      <c r="F2" s="6">
+        <v>44307</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3">
+        <v>44452</v>
+      </c>
+      <c r="F3" s="3">
         <v>44521</v>
       </c>
-      <c r="E2">
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3">
+        <v>44489</v>
+      </c>
+      <c r="F4" s="3">
+        <v>44499</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="3">
+        <v>44510</v>
+      </c>
+      <c r="F5" s="3">
+        <v>44515</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3">
+        <v>44516</v>
+      </c>
+      <c r="F6" s="3">
+        <v>44520</v>
+      </c>
+      <c r="G6">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3">
-        <v>44452</v>
-      </c>
-      <c r="D3" s="3">
-        <v>44521</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4432D9D-587E-488B-88B4-D4CEF7C3FEB7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="B15:D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3">
+        <v>44497</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>44306</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>44496</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
+        <v>44307</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>44515</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>44516</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3">
+        <v>44514</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>44520</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>44519</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
displays data inserted into the database
Co-Authored-By: Lucas Briz <73654573+lucasbriz@users.noreply.github.com>
Co-Authored-By: karinkagi <95055760+karinkagi@users.noreply.github.com>
Co-Authored-By: Mateus Moraes Toledo <95055897+mateus11toledo@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/insertData.xlsx
+++ b/insertData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luana.scardua\Downloads\SQLite-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luana\Documents\SQLite-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CC5882-366A-4A8B-B41B-6FAFAA5178A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD60F51-605D-409E-9AC1-A5187D657702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6CFF9A66-05E6-4823-8BFA-658619B48BFB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{6CFF9A66-05E6-4823-8BFA-658619B48BFB}"/>
   </bookViews>
   <sheets>
     <sheet name="usuario" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="avaliacao" sheetId="4" r:id="rId3"/>
     <sheet name="avaliacaoAluno" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>id</t>
   </si>
@@ -89,6 +89,24 @@
   </si>
   <si>
     <t>PROJ</t>
+  </si>
+  <si>
+    <t>ID User</t>
+  </si>
+  <si>
+    <t>ID Avaliação</t>
+  </si>
+  <si>
+    <t>data conclusão</t>
+  </si>
+  <si>
+    <t>nota</t>
+  </si>
+  <si>
+    <t>situação</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -451,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F016AF-984E-4592-8A35-D09FFCDCC7C2}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -462,7 +480,7 @@
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,11 +493,13 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -490,7 +510,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -509,23 +529,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F405A2-8FE6-4448-B6F8-DFECE18E1EBE}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -533,7 +556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -549,80 +572,114 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E4AC80-24BD-4308-9E1D-510E74F54FEE}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44256</v>
+      </c>
+      <c r="E2" s="3">
+        <v>44521</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44452</v>
+      </c>
+      <c r="E3" s="3">
+        <v>44521</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4432D9D-587E-488B-88B4-D4CEF7C3FEB7}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3">
-        <v>44256</v>
-      </c>
-      <c r="D2" s="3">
-        <v>44521</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3">
-        <v>44452</v>
-      </c>
-      <c r="D3" s="3">
-        <v>44521</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4432D9D-587E-488B-88B4-D4CEF7C3FEB7}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>